<commit_message>
trying to fit with lognormal
</commit_message>
<xml_diff>
--- a/Data/correlation matrix.xlsx
+++ b/Data/correlation matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazak\PycharmProjects\pythonProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazak\PycharmProjects\Assembly_data_processing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C49C0F0-B88B-47E2-B9D9-3D0F9CFA299E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B37CD-EEB9-42AE-A7AA-6B096C6751F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>r1</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>B-4</t>
+  </si>
+  <si>
+    <t>Hook_con</t>
+  </si>
+  <si>
+    <t>Hook_type</t>
+  </si>
+  <si>
+    <t>Hook_uncon</t>
   </si>
 </sst>
 </file>
@@ -151,14 +160,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -243,43 +253,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -303,11 +276,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,31 +330,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P6"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -664,41 +640,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="16" t="s">
@@ -731,50 +707,50 @@
       <c r="O2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="3">
         <v>7</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="3">
         <v>14</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="16">
-        <v>-0.18762974159883999</v>
-      </c>
-      <c r="F3" s="16">
-        <v>-0.12257557786523</v>
-      </c>
-      <c r="G3" s="16">
-        <v>0.13911306116840599</v>
-      </c>
-      <c r="H3" s="16">
-        <v>-0.134787013065538</v>
-      </c>
-      <c r="I3" s="16">
-        <v>-0.143432442004952</v>
-      </c>
-      <c r="J3" s="16">
-        <v>-0.25851065283303798</v>
-      </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="16">
-        <v>-0.179699723200519</v>
-      </c>
-      <c r="P3" s="17">
-        <v>-0.13954976049097401</v>
+      <c r="E3" s="9">
+        <v>-0.191859995073727</v>
+      </c>
+      <c r="F3" s="10">
+        <v>-0.12050678256330299</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.13400814691737201</v>
+      </c>
+      <c r="H3" s="10">
+        <v>-0.13145465383994401</v>
+      </c>
+      <c r="I3" s="10">
+        <v>-6.1564585609429699E-2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>-0.21913008410113599</v>
+      </c>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="10">
+        <v>-0.113491787334735</v>
+      </c>
+      <c r="P3" s="11">
+        <v>-6.1191042336295499E-2</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -790,41 +766,41 @@
       <c r="D4" s="4">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
-        <v>-5.1099273556603098E-2</v>
+      <c r="E4" s="2">
+        <v>-0.10172480917256101</v>
       </c>
       <c r="F4" s="3">
-        <v>-0.160048703537996</v>
+        <v>-0.14396238497102001</v>
       </c>
       <c r="G4" s="3">
-        <v>-6.0084233143380301E-2</v>
+        <v>-0.159528604377599</v>
       </c>
       <c r="H4" s="3">
-        <v>-5.2638786645951702E-2</v>
+        <v>-7.9704962494216103E-2</v>
       </c>
       <c r="I4" s="3">
-        <v>2.0168141748665502E-2</v>
+        <v>-1.6673009220201099E-2</v>
       </c>
       <c r="J4" s="3">
-        <v>-9.94928546588211E-2</v>
+        <v>-4.4881918074529603E-3</v>
       </c>
       <c r="K4" s="3">
-        <v>9.3162759532042103E-2</v>
+        <v>1.02547399049659E-2</v>
       </c>
       <c r="L4" s="3">
-        <v>-0.118181852093937</v>
+        <v>8.5420834958091999E-3</v>
       </c>
       <c r="M4" s="3">
-        <v>0.225700806632878</v>
+        <v>6.1480793102851101E-2</v>
       </c>
       <c r="N4" s="3">
-        <v>-0.27566226653419101</v>
+        <v>-6.7474400059471695E-2</v>
       </c>
       <c r="O4" s="3">
-        <v>-9.5875225241111306E-3</v>
+        <v>-4.2906147896802901E-2</v>
       </c>
       <c r="P4" s="4">
-        <v>3.42851928833596E-2</v>
+        <v>-7.1944808879156594E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -840,33 +816,33 @@
       <c r="D5" s="4">
         <v>6</v>
       </c>
-      <c r="E5" s="3">
-        <v>-0.11862216838617699</v>
+      <c r="E5" s="2">
+        <v>-0.14948791852972301</v>
       </c>
       <c r="F5" s="3">
-        <v>-0.14054433436195399</v>
-      </c>
-      <c r="G5" s="3">
-        <v>4.1716302879347598E-2</v>
+        <v>-0.106662710595839</v>
+      </c>
+      <c r="G5" s="14">
+        <v>-0.22349079768573399</v>
       </c>
       <c r="H5" s="3">
-        <v>-0.13898907175255701</v>
+        <v>-7.5580890251431096E-2</v>
       </c>
       <c r="I5" s="3">
-        <v>9.54271915936315E-2</v>
+        <v>-3.39997765327478E-2</v>
       </c>
       <c r="J5" s="3">
-        <v>-5.3634814423434901E-2</v>
+        <v>1.48564140955994E-2</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="3">
-        <v>-3.5227534681544902E-2</v>
+        <v>-0.117419365429436</v>
       </c>
       <c r="P5" s="4">
-        <v>9.0418780149932598E-3</v>
+        <v>-6.9167704316348999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -882,35 +858,122 @@
       <c r="D6" s="7">
         <v>4</v>
       </c>
-      <c r="E6" s="6">
-        <v>-0.25717161419298601</v>
-      </c>
-      <c r="F6" s="19">
-        <v>-0.29445088383854401</v>
+      <c r="E6" s="5">
+        <v>-9.5695524343472199E-2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>-0.13758548668267601</v>
       </c>
       <c r="G6" s="6">
-        <v>-0.178342215727194</v>
+        <v>-7.5523350862626196E-2</v>
       </c>
       <c r="H6" s="6">
-        <v>-0.18202461490267699</v>
-      </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
+        <v>-3.9801376011293702E-2</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
       <c r="O6" s="6">
-        <v>-0.27517156168228502</v>
+        <v>-0.109761074639193</v>
       </c>
       <c r="P6" s="7">
-        <v>-0.17293494405626</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="L9" s="1" cm="1">
-        <f t="array" ref="L9">MAX(ABS((E3:N4)))</f>
-        <v>0.27566226653419101</v>
+        <v>-0.12478342114341399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="I11" s="1" cm="1">
+        <f t="array" ref="I11">MAX(ABS(E3:P6))</f>
+        <v>0.22349079768573399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.17417392070243901</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.102340253017347</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.196141822507752</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="3">
+        <v>0.16321778114198501</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0.16213309459349401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="6">
+        <v>1.36212440288258E-2</v>
+      </c>
+      <c r="C14" s="6">
+        <v>7.2568994006718497E-3</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2.5705424127807699E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-5.4368667957803103E-2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>-0.101860819383187</v>
+      </c>
+      <c r="G14" s="6">
+        <v>-2.9018359765971499E-2</v>
+      </c>
+      <c r="H14" s="6">
+        <v>-2.97194641903781E-2</v>
+      </c>
+      <c r="I14" s="7">
+        <v>-2.29715417959678E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="1" cm="1">
+        <f t="array" ref="F17">MAX(ABS(B13:I14))</f>
+        <v>0.196141822507752</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +981,7 @@
     <mergeCell ref="E1:P1"/>
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>